<commit_message>
CHISA Fighting... a lot of changes in optimization a loss functions calculations
</commit_message>
<xml_diff>
--- a/docu/tmp/TestExperiment3.xlsx
+++ b/docu/tmp/TestExperiment3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABF3D15-21F0-49E8-865A-23C239CE3200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB63093-0B96-4424-952E-C5358016F603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="1515" windowWidth="16155" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33855" yWindow="-2835" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -817,7 +817,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1097,16 +1097,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1114,12 +1114,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1128,12 +1128,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1142,7 +1142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>44496</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1167,8 +1167,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>0</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>4</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>6</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>8</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>10</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>12</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>11.222</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>13.787000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>15.542999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>20</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>15.542</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>22</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>14.292</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>24</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>12.627000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>26</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>10.003</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>28</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>30</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>32</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>34</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>36</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>38</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>40</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>45</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>50</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>55</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>60</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>65</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>70</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>75</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>80</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>85</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>90</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>105</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>120</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>135</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>150</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>165</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7">
         <v>180</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>